<commit_message>
Budget Example 1 + Design
Test Example For A User - still in progress
</commit_message>
<xml_diff>
--- a/blb_content/Expenses/Expense Data Outline.xlsx
+++ b/blb_content/Expenses/Expense Data Outline.xlsx
@@ -5,19 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/555b4b563df01d52/Bottom Line Budgeting/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kolin\Documents\GitHub\budget-app\blb_content\Expenses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="8_{266591FF-9276-4E9B-99F3-F153A76E4803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB2D6E76-EF3A-477C-AC0C-1A24A543CBF9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B474DD9-EB73-4341-923A-03A5680B05EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C275CF63-FFB3-4A38-90CF-B958D3806680}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{C275CF63-FFB3-4A38-90CF-B958D3806680}"/>
   </bookViews>
   <sheets>
-    <sheet name="Discretionary Expenses" sheetId="1" r:id="rId1"/>
-    <sheet name="Reocurring Expenses" sheetId="2" r:id="rId2"/>
+    <sheet name="DB_Discretionary Expenses" sheetId="1" r:id="rId1"/>
+    <sheet name="DB_Reocurring Expenses" sheetId="2" r:id="rId2"/>
+    <sheet name="Side Bar Design" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Discretionary Expenses'!$F$1:$F$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'DB_Discretionary Expenses'!$F$1:$F$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -92,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="59">
   <si>
     <t>Month</t>
   </si>
@@ -257,13 +258,25 @@
   </si>
   <si>
     <t>Renters Insurance</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>2021 Overview</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year </t>
+  </si>
+  <si>
+    <t>Budget Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,14 +299,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -343,7 +366,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -397,18 +420,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -416,22 +460,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="6" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="5" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="8"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="9"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="11">
     <cellStyle name="20% - Accent2" xfId="2" builtinId="34"/>
     <cellStyle name="20% - Accent4" xfId="3" builtinId="42"/>
     <cellStyle name="20% - Accent5" xfId="5" builtinId="46"/>
     <cellStyle name="20% - Accent6" xfId="7" builtinId="50"/>
     <cellStyle name="40% - Accent4" xfId="4" builtinId="43"/>
     <cellStyle name="60% - Accent5" xfId="6" builtinId="48"/>
+    <cellStyle name="Heading 1" xfId="8" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="9" builtinId="17"/>
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="10" builtinId="19"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -796,7 +846,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,8 +1167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93986363-349C-4DC2-A148-9F4BACB53A99}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1358,4 +1408,111 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8213353-3C95-474C-9F2E-7BEC71FAEFCB}">
+  <dimension ref="A1:A27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="12"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="12"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="12"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>